<commit_message>
Update Pianificazione eventi RLadies.xlsx
</commit_message>
<xml_diff>
--- a/Pianificazione eventi RLadies.xlsx
+++ b/Pianificazione eventi RLadies.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RLadies\meetup-presentations_bari\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\RLadies\meetup-presentations_bari\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>PIANIFICAZIONE MENSILE</t>
   </si>
@@ -139,7 +139,10 @@
     <t>EVENTI COMUNITÀ</t>
   </si>
   <si>
-    <t>Introduction to R - Giovanna de Vincenzo</t>
+    <t>Primi passi in Rstudio - Francesca</t>
+  </si>
+  <si>
+    <t>Manipolare i dati con Tidyverse</t>
   </si>
 </sst>
 </file>
@@ -797,6 +800,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="22" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -823,15 +835,6 @@
     </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2499,7 +2502,7 @@
   <dimension ref="B1:M15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2531,7 +2534,7 @@
     </row>
     <row r="4" spans="2:13" ht="14.25" x14ac:dyDescent="0.2"/>
     <row r="5" spans="2:13" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M5" s="97"/>
+      <c r="M5" s="88"/>
     </row>
     <row r="6" spans="2:13" ht="69" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -2551,11 +2554,11 @@
     </row>
     <row r="9" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
-        <v>43479</v>
+        <v>43494</v>
       </c>
       <c r="C9" s="6" t="str">
         <f>IF(ISBLANK(tblEventi[[#This Row],[DATA]]),"",UPPER(TEXT(tblEventi[[#This Row],[DATA]],"ggg")))</f>
-        <v>LUN</v>
+        <v>MAR</v>
       </c>
       <c r="D9" s="6" t="str">
         <f>IF(ISBLANK(tblEventi[[#This Row],[DATA]]),"",UPPER(TEXT(tblEventi[[#This Row],[DATA]],"mmm")))</f>
@@ -2567,17 +2570,19 @@
     </row>
     <row r="10" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
-        <v>43500</v>
+        <v>43529</v>
       </c>
       <c r="C10" s="6" t="str">
         <f>IF(ISBLANK(tblEventi[[#This Row],[DATA]]),"",UPPER(TEXT(tblEventi[[#This Row],[DATA]],"ggg")))</f>
-        <v>LUN</v>
+        <v>MAR</v>
       </c>
       <c r="D10" s="6" t="str">
         <f>IF(ISBLANK(tblEventi[[#This Row],[DATA]]),"",UPPER(TEXT(tblEventi[[#This Row],[DATA]],"mmm")))</f>
-        <v>FEB</v>
-      </c>
-      <c r="E10" s="7"/>
+        <v>MAR</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
@@ -2639,15 +2644,15 @@
       <c r="B15" s="5">
         <v>43647</v>
       </c>
-      <c r="C15" s="98" t="str">
+      <c r="C15" s="89" t="str">
         <f>IF(ISBLANK(tblEventi[[#This Row],[DATA]]),"",UPPER(TEXT(tblEventi[[#This Row],[DATA]],"ggg")))</f>
         <v>LUN</v>
       </c>
-      <c r="D15" s="98" t="str">
+      <c r="D15" s="89" t="str">
         <f>IF(ISBLANK(tblEventi[[#This Row],[DATA]]),"",UPPER(TEXT(tblEventi[[#This Row],[DATA]],"mmm")))</f>
         <v>LUG</v>
       </c>
-      <c r="E15" s="99"/>
+      <c r="E15" s="90"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -2708,16 +2713,16 @@
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
-      <c r="F2" s="89" t="str">
+      <c r="F2" s="92" t="str">
         <f>LOOKUP(NumMese,tblMesi[NUMERO],tblMesi[MESE])</f>
         <v>GENNAIO</v>
       </c>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
       <c r="M2" s="11"/>
       <c r="N2" s="11"/>
       <c r="O2" s="11"/>
@@ -3304,7 +3309,7 @@
       <c r="B17" s="8"/>
       <c r="C17" s="78" t="str">
         <f t="array" ref="C17">IFERROR(INDEX(tblEventi[],SMALL(IF(Date=C$16,ROW(Date)),ROW(1:1))-InizioRigaTabella,4),"")</f>
-        <v>Introduction to R - Giovanna de Vincenzo</v>
+        <v/>
       </c>
       <c r="D17" s="78"/>
       <c r="E17" s="79"/>
@@ -3750,7 +3755,7 @@
       <c r="E27" s="79"/>
       <c r="F27" s="79" t="str">
         <f t="array" ref="F27">IFERROR(INDEX(tblEventi[],SMALL(IF(Date=F$26,ROW(Date)),ROW(1:1))-InizioRigaTabella,4),"")</f>
-        <v/>
+        <v>Primi passi in Rstudio - Francesca</v>
       </c>
       <c r="G27" s="79"/>
       <c r="H27" s="80"/>
@@ -3930,28 +3935,28 @@
       </c>
       <c r="G31" s="14"/>
       <c r="H31" s="46"/>
-      <c r="I31" s="88" t="s">
+      <c r="I31" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="J31" s="88"/>
-      <c r="K31" s="88"/>
-      <c r="L31" s="88"/>
-      <c r="M31" s="88"/>
-      <c r="N31" s="88"/>
-      <c r="O31" s="88"/>
-      <c r="P31" s="88"/>
-      <c r="Q31" s="88"/>
-      <c r="R31" s="88"/>
-      <c r="S31" s="88"/>
-      <c r="T31" s="88"/>
-      <c r="U31" s="88"/>
+      <c r="J31" s="91"/>
+      <c r="K31" s="91"/>
+      <c r="L31" s="91"/>
+      <c r="M31" s="91"/>
+      <c r="N31" s="91"/>
+      <c r="O31" s="91"/>
+      <c r="P31" s="91"/>
+      <c r="Q31" s="91"/>
+      <c r="R31" s="91"/>
+      <c r="S31" s="91"/>
+      <c r="T31" s="91"/>
+      <c r="U31" s="91"/>
       <c r="V31" s="73"/>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B32" s="8"/>
-      <c r="C32" s="78">
+      <c r="C32" s="78" t="str">
         <f t="array" ref="C32">IFERROR(INDEX(tblEventi[],SMALL(IF(Date=C$31,ROW(Date)),ROW(1:1))-InizioRigaTabella,4),"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D32" s="78"/>
       <c r="E32" s="79"/>
@@ -3961,19 +3966,19 @@
       </c>
       <c r="G32" s="15"/>
       <c r="H32" s="47"/>
-      <c r="I32" s="88"/>
-      <c r="J32" s="88"/>
-      <c r="K32" s="88"/>
-      <c r="L32" s="88"/>
-      <c r="M32" s="88"/>
-      <c r="N32" s="88"/>
-      <c r="O32" s="88"/>
-      <c r="P32" s="88"/>
-      <c r="Q32" s="88"/>
-      <c r="R32" s="88"/>
-      <c r="S32" s="88"/>
-      <c r="T32" s="88"/>
-      <c r="U32" s="88"/>
+      <c r="I32" s="91"/>
+      <c r="J32" s="91"/>
+      <c r="K32" s="91"/>
+      <c r="L32" s="91"/>
+      <c r="M32" s="91"/>
+      <c r="N32" s="91"/>
+      <c r="O32" s="91"/>
+      <c r="P32" s="91"/>
+      <c r="Q32" s="91"/>
+      <c r="R32" s="91"/>
+      <c r="S32" s="91"/>
+      <c r="T32" s="91"/>
+      <c r="U32" s="91"/>
       <c r="V32" s="74"/>
     </row>
     <row r="33" spans="2:22" x14ac:dyDescent="0.2">
@@ -3990,19 +3995,19 @@
       </c>
       <c r="G33" s="15"/>
       <c r="H33" s="47"/>
-      <c r="I33" s="88"/>
-      <c r="J33" s="88"/>
-      <c r="K33" s="88"/>
-      <c r="L33" s="88"/>
-      <c r="M33" s="88"/>
-      <c r="N33" s="88"/>
-      <c r="O33" s="88"/>
-      <c r="P33" s="88"/>
-      <c r="Q33" s="88"/>
-      <c r="R33" s="88"/>
-      <c r="S33" s="88"/>
-      <c r="T33" s="88"/>
-      <c r="U33" s="88"/>
+      <c r="I33" s="91"/>
+      <c r="J33" s="91"/>
+      <c r="K33" s="91"/>
+      <c r="L33" s="91"/>
+      <c r="M33" s="91"/>
+      <c r="N33" s="91"/>
+      <c r="O33" s="91"/>
+      <c r="P33" s="91"/>
+      <c r="Q33" s="91"/>
+      <c r="R33" s="91"/>
+      <c r="S33" s="91"/>
+      <c r="T33" s="91"/>
+      <c r="U33" s="91"/>
       <c r="V33" s="74"/>
     </row>
     <row r="34" spans="2:22" x14ac:dyDescent="0.2">
@@ -4019,19 +4024,19 @@
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="47"/>
-      <c r="I34" s="88"/>
-      <c r="J34" s="88"/>
-      <c r="K34" s="88"/>
-      <c r="L34" s="88"/>
-      <c r="M34" s="88"/>
-      <c r="N34" s="88"/>
-      <c r="O34" s="88"/>
-      <c r="P34" s="88"/>
-      <c r="Q34" s="88"/>
-      <c r="R34" s="88"/>
-      <c r="S34" s="88"/>
-      <c r="T34" s="88"/>
-      <c r="U34" s="88"/>
+      <c r="I34" s="91"/>
+      <c r="J34" s="91"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="91"/>
+      <c r="M34" s="91"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="91"/>
+      <c r="P34" s="91"/>
+      <c r="Q34" s="91"/>
+      <c r="R34" s="91"/>
+      <c r="S34" s="91"/>
+      <c r="T34" s="91"/>
+      <c r="U34" s="91"/>
       <c r="V34" s="74"/>
     </row>
     <row r="35" spans="2:22" x14ac:dyDescent="0.2">
@@ -4048,19 +4053,19 @@
       </c>
       <c r="G35" s="15"/>
       <c r="H35" s="47"/>
-      <c r="I35" s="88"/>
-      <c r="J35" s="88"/>
-      <c r="K35" s="88"/>
-      <c r="L35" s="88"/>
-      <c r="M35" s="88"/>
-      <c r="N35" s="88"/>
-      <c r="O35" s="88"/>
-      <c r="P35" s="88"/>
-      <c r="Q35" s="88"/>
-      <c r="R35" s="88"/>
-      <c r="S35" s="88"/>
-      <c r="T35" s="88"/>
-      <c r="U35" s="88"/>
+      <c r="I35" s="91"/>
+      <c r="J35" s="91"/>
+      <c r="K35" s="91"/>
+      <c r="L35" s="91"/>
+      <c r="M35" s="91"/>
+      <c r="N35" s="91"/>
+      <c r="O35" s="91"/>
+      <c r="P35" s="91"/>
+      <c r="Q35" s="91"/>
+      <c r="R35" s="91"/>
+      <c r="S35" s="91"/>
+      <c r="T35" s="91"/>
+      <c r="U35" s="91"/>
       <c r="V35" s="74"/>
     </row>
   </sheetData>
@@ -4169,26 +4174,26 @@
       </c>
       <c r="D2" s="50"/>
       <c r="E2" s="50"/>
-      <c r="F2" s="90" t="str">
+      <c r="F2" s="93" t="str">
         <f>VisualizzazioneMese</f>
         <v>GENNAIO</v>
       </c>
-      <c r="G2" s="90">
-        <v>0</v>
-      </c>
-      <c r="H2" s="90">
-        <v>0</v>
-      </c>
-      <c r="I2" s="90">
-        <v>0</v>
-      </c>
-      <c r="J2" s="90">
-        <v>0</v>
-      </c>
-      <c r="K2" s="90">
-        <v>0</v>
-      </c>
-      <c r="L2" s="90">
+      <c r="G2" s="93">
+        <v>0</v>
+      </c>
+      <c r="H2" s="93">
+        <v>0</v>
+      </c>
+      <c r="I2" s="93">
+        <v>0</v>
+      </c>
+      <c r="J2" s="93">
+        <v>0</v>
+      </c>
+      <c r="K2" s="93">
+        <v>0</v>
+      </c>
+      <c r="L2" s="93">
         <v>0</v>
       </c>
       <c r="M2" s="51"/>
@@ -5151,7 +5156,7 @@
       <c r="B17" s="61"/>
       <c r="C17" s="61" t="str">
         <f>CALENDARIO!C17</f>
-        <v>Introduction to R - Giovanna de Vincenzo</v>
+        <v/>
       </c>
       <c r="D17" s="61">
         <f>CALENDARIO!D17</f>
@@ -5963,7 +5968,7 @@
       </c>
       <c r="F27" s="61" t="str">
         <f>CALENDARIO!F27</f>
-        <v/>
+        <v>Primi passi in Rstudio - Francesca</v>
       </c>
       <c r="G27" s="61">
         <f>CALENDARIO!G27</f>
@@ -6287,29 +6292,29 @@
       </c>
       <c r="G31" s="61"/>
       <c r="H31" s="65"/>
-      <c r="I31" s="91" t="str">
+      <c r="I31" s="94" t="str">
         <f>CALENDARIO!I31</f>
         <v>NOTE:</v>
       </c>
-      <c r="J31" s="91"/>
-      <c r="K31" s="91"/>
-      <c r="L31" s="91"/>
-      <c r="M31" s="91"/>
-      <c r="N31" s="91"/>
-      <c r="O31" s="91"/>
-      <c r="P31" s="91"/>
-      <c r="Q31" s="91"/>
-      <c r="R31" s="91"/>
-      <c r="S31" s="91"/>
-      <c r="T31" s="91"/>
-      <c r="U31" s="92"/>
+      <c r="J31" s="94"/>
+      <c r="K31" s="94"/>
+      <c r="L31" s="94"/>
+      <c r="M31" s="94"/>
+      <c r="N31" s="94"/>
+      <c r="O31" s="94"/>
+      <c r="P31" s="94"/>
+      <c r="Q31" s="94"/>
+      <c r="R31" s="94"/>
+      <c r="S31" s="94"/>
+      <c r="T31" s="94"/>
+      <c r="U31" s="95"/>
       <c r="V31" s="61"/>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B32" s="58"/>
-      <c r="C32" s="61">
+      <c r="C32" s="61" t="str">
         <f>CALENDARIO!C32</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D32" s="61">
         <f>CALENDARIO!D32</f>
@@ -6325,19 +6330,19 @@
       </c>
       <c r="G32" s="58"/>
       <c r="H32" s="66"/>
-      <c r="I32" s="93"/>
-      <c r="J32" s="93"/>
-      <c r="K32" s="93"/>
-      <c r="L32" s="93"/>
-      <c r="M32" s="93"/>
-      <c r="N32" s="93"/>
-      <c r="O32" s="93"/>
-      <c r="P32" s="93"/>
-      <c r="Q32" s="93"/>
-      <c r="R32" s="93"/>
-      <c r="S32" s="93"/>
-      <c r="T32" s="93"/>
-      <c r="U32" s="94"/>
+      <c r="I32" s="96"/>
+      <c r="J32" s="96"/>
+      <c r="K32" s="96"/>
+      <c r="L32" s="96"/>
+      <c r="M32" s="96"/>
+      <c r="N32" s="96"/>
+      <c r="O32" s="96"/>
+      <c r="P32" s="96"/>
+      <c r="Q32" s="96"/>
+      <c r="R32" s="96"/>
+      <c r="S32" s="96"/>
+      <c r="T32" s="96"/>
+      <c r="U32" s="97"/>
       <c r="V32" s="58"/>
     </row>
     <row r="33" spans="2:22" x14ac:dyDescent="0.2">
@@ -6360,19 +6365,19 @@
       </c>
       <c r="G33" s="60"/>
       <c r="H33" s="67"/>
-      <c r="I33" s="93"/>
-      <c r="J33" s="93"/>
-      <c r="K33" s="93"/>
-      <c r="L33" s="93"/>
-      <c r="M33" s="93"/>
-      <c r="N33" s="93"/>
-      <c r="O33" s="93"/>
-      <c r="P33" s="93"/>
-      <c r="Q33" s="93"/>
-      <c r="R33" s="93"/>
-      <c r="S33" s="93"/>
-      <c r="T33" s="93"/>
-      <c r="U33" s="94"/>
+      <c r="I33" s="96"/>
+      <c r="J33" s="96"/>
+      <c r="K33" s="96"/>
+      <c r="L33" s="96"/>
+      <c r="M33" s="96"/>
+      <c r="N33" s="96"/>
+      <c r="O33" s="96"/>
+      <c r="P33" s="96"/>
+      <c r="Q33" s="96"/>
+      <c r="R33" s="96"/>
+      <c r="S33" s="96"/>
+      <c r="T33" s="96"/>
+      <c r="U33" s="97"/>
       <c r="V33" s="60"/>
     </row>
     <row r="34" spans="2:22" x14ac:dyDescent="0.2">
@@ -6395,19 +6400,19 @@
       </c>
       <c r="G34" s="60"/>
       <c r="H34" s="67"/>
-      <c r="I34" s="93"/>
-      <c r="J34" s="93"/>
-      <c r="K34" s="93"/>
-      <c r="L34" s="93"/>
-      <c r="M34" s="93"/>
-      <c r="N34" s="93"/>
-      <c r="O34" s="93"/>
-      <c r="P34" s="93"/>
-      <c r="Q34" s="93"/>
-      <c r="R34" s="93"/>
-      <c r="S34" s="93"/>
-      <c r="T34" s="93"/>
-      <c r="U34" s="94"/>
+      <c r="I34" s="96"/>
+      <c r="J34" s="96"/>
+      <c r="K34" s="96"/>
+      <c r="L34" s="96"/>
+      <c r="M34" s="96"/>
+      <c r="N34" s="96"/>
+      <c r="O34" s="96"/>
+      <c r="P34" s="96"/>
+      <c r="Q34" s="96"/>
+      <c r="R34" s="96"/>
+      <c r="S34" s="96"/>
+      <c r="T34" s="96"/>
+      <c r="U34" s="97"/>
       <c r="V34" s="60"/>
     </row>
     <row r="35" spans="2:22" x14ac:dyDescent="0.2">
@@ -6430,19 +6435,19 @@
       </c>
       <c r="G35" s="60"/>
       <c r="H35" s="68"/>
-      <c r="I35" s="95"/>
-      <c r="J35" s="95"/>
-      <c r="K35" s="95"/>
-      <c r="L35" s="95"/>
-      <c r="M35" s="95"/>
-      <c r="N35" s="95"/>
-      <c r="O35" s="95"/>
-      <c r="P35" s="95"/>
-      <c r="Q35" s="95"/>
-      <c r="R35" s="95"/>
-      <c r="S35" s="95"/>
-      <c r="T35" s="95"/>
-      <c r="U35" s="96"/>
+      <c r="I35" s="98"/>
+      <c r="J35" s="98"/>
+      <c r="K35" s="98"/>
+      <c r="L35" s="98"/>
+      <c r="M35" s="98"/>
+      <c r="N35" s="98"/>
+      <c r="O35" s="98"/>
+      <c r="P35" s="98"/>
+      <c r="Q35" s="98"/>
+      <c r="R35" s="98"/>
+      <c r="S35" s="98"/>
+      <c r="T35" s="98"/>
+      <c r="U35" s="99"/>
       <c r="V35" s="60"/>
     </row>
   </sheetData>

</xml_diff>